<commit_message>
deceived v. non-deceived stats
</commit_message>
<xml_diff>
--- a/derivatives/palm_data/data/act_domain_x_outcome.xlsx
+++ b/derivatives/palm_data/data/act_domain_x_outcome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/Documents_Air/GitHub/istart-socdoors/derivatives/palm_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2632C27A-CE4A-DC49-97C6-D1018DE7D0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FF1FCF1B-BB11-C44D-A281-DF467539F254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,16 +36,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1" uniqueCount="1">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2" uniqueCount="2">
   <si>
     <t>act</t>
+  </si>
+  <si>
+    <t>sub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -179,6 +182,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -522,8 +531,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -899,234 +909,371 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A45"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B2">
         <v>16.460726000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B3">
         <v>-11.036606000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B4">
         <v>-51.199348999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1006</v>
+      </c>
+      <c r="B5">
         <v>125.66677900000001</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1009</v>
+      </c>
+      <c r="B6">
         <v>19.759650000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1010</v>
+      </c>
+      <c r="B7">
         <v>15.988225999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1012</v>
+      </c>
+      <c r="B8">
         <v>-38.344462999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1013</v>
+      </c>
+      <c r="B9">
         <v>-40.676152000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1015</v>
+      </c>
+      <c r="B10">
         <v>5.2040850000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1016</v>
+      </c>
+      <c r="B11">
         <v>48.876719999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1019</v>
+      </c>
+      <c r="B12">
         <v>-38.531056</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1021</v>
+      </c>
+      <c r="B13">
         <v>-22.450993</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1242</v>
+      </c>
+      <c r="B14">
         <v>-42.164495000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1243</v>
+      </c>
+      <c r="B15">
         <v>6.527012</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1244</v>
+      </c>
+      <c r="B16">
         <v>-38.664344</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1245</v>
+      </c>
+      <c r="B17">
         <v>-59.178106</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>1247</v>
+      </c>
+      <c r="B18">
         <v>-26.603785999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>1248</v>
+      </c>
+      <c r="B19">
         <v>-28.278022</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1249</v>
+      </c>
+      <c r="B20">
         <v>-8.3417429999999992</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1251</v>
+      </c>
+      <c r="B21">
         <v>-164.17443599999999</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>1255</v>
+      </c>
+      <c r="B22">
         <v>-24.33785</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>1276</v>
+      </c>
+      <c r="B23">
         <v>-3.3622420000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>1286</v>
+      </c>
+      <c r="B24">
         <v>4.348179</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>1294</v>
+      </c>
+      <c r="B25">
         <v>-13.111482000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>1301</v>
+      </c>
+      <c r="B26">
         <v>74.057562000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>1302</v>
+      </c>
+      <c r="B27">
         <v>25.155227</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>1303</v>
+      </c>
+      <c r="B28">
         <v>-9.6269089999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>3116</v>
+      </c>
+      <c r="B29">
         <v>-42.021005000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>3122</v>
+      </c>
+      <c r="B30">
         <v>61.805723</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>3125</v>
+      </c>
+      <c r="B31">
         <v>-45.427199000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>3140</v>
+      </c>
+      <c r="B32">
         <v>-5.8167809999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>3143</v>
+      </c>
+      <c r="B33">
         <v>-73.16968</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>3166</v>
+      </c>
+      <c r="B34">
         <v>-21.134269</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>3167</v>
+      </c>
+      <c r="B35">
         <v>9.074738</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>3170</v>
+      </c>
+      <c r="B36">
         <v>56.439529999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>3173</v>
+      </c>
+      <c r="B37">
         <v>5.9932400000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>3175</v>
+      </c>
+      <c r="B38">
         <v>-6.1108409999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>3176</v>
+      </c>
+      <c r="B39">
         <v>-39.381563999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>3189</v>
+      </c>
+      <c r="B40">
         <v>91.250421000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>3190</v>
+      </c>
+      <c r="B41">
         <v>-44.097996000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>3200</v>
+      </c>
+      <c r="B42">
         <v>-11.310219999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>3206</v>
+      </c>
+      <c r="B43">
         <v>-13.598561999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>3212</v>
+      </c>
+      <c r="B44">
         <v>76.326590999999993</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>3220</v>
+      </c>
+      <c r="B45">
         <v>22.642925999999999</v>
       </c>
     </row>

</xml_diff>